<commit_message>
update NPP error propogation
</commit_message>
<xml_diff>
--- a/Complete_the_carbon_cycle/Error_propogation/trait_NPP_ghana_organized.xlsx
+++ b/Complete_the_carbon_cycle/Error_propogation/trait_NPP_ghana_organized.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Oxford\Chapter_two\Complete_the_carbon_cycle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B02B1A2-1A65-43DC-9154-0A07B5924A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7932F36-BD39-4B06-B288-E8A094FF00D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28110" yWindow="-21690" windowWidth="25820" windowHeight="38620" activeTab="3" xr2:uid="{9F852EB7-8A5A-4C4B-A58A-D6B1E4E3EF65}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="117">
   <si>
     <t>BOB02-T391-B01S-L01aci_May_15_.txt</t>
   </si>
@@ -361,6 +361,60 @@
   </si>
   <si>
     <t>NPP_BG</t>
+  </si>
+  <si>
+    <t>NPP_canopy_se</t>
+  </si>
+  <si>
+    <t>NPP_leaf_se</t>
+  </si>
+  <si>
+    <t>NPP_twigs_se</t>
+  </si>
+  <si>
+    <t>NPP_flower_se</t>
+  </si>
+  <si>
+    <t>NPP_fruit_se</t>
+  </si>
+  <si>
+    <t>NPP_unidentified_se</t>
+  </si>
+  <si>
+    <t>NPP_seed_se</t>
+  </si>
+  <si>
+    <t>NPP_herbivory_se</t>
+  </si>
+  <si>
+    <t>NPP_branch_turnover_se</t>
+  </si>
+  <si>
+    <t>NPPacw_10cm_big_stem_se</t>
+  </si>
+  <si>
+    <t>NPPacw_small_stem_se</t>
+  </si>
+  <si>
+    <t>NPP_all_stem_se</t>
+  </si>
+  <si>
+    <t>NPP_coarseroot_se</t>
+  </si>
+  <si>
+    <t>NPP_fineroot_se</t>
+  </si>
+  <si>
+    <t>NPP_herbs_se</t>
+  </si>
+  <si>
+    <t>NPP_AG_se</t>
+  </si>
+  <si>
+    <t>NPP_BG_se</t>
+  </si>
+  <si>
+    <t>NPP_se</t>
   </si>
 </sst>
 </file>
@@ -3799,13 +3853,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="I1:I2"/>
     <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="AC1:AC2"/>
     <mergeCell ref="O1:O2"/>
@@ -3814,6 +3861,13 @@
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3825,7 +3879,7 @@
   <dimension ref="A1:AK15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3891,77 +3945,59 @@
       <c r="S1" t="s">
         <v>39</v>
       </c>
-      <c r="T1" t="str">
-        <f t="shared" ref="T1:AK1" si="0">_xlfn.CONCAT("d",B1)</f>
-        <v>dNPP_canopy</v>
-      </c>
-      <c r="U1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP_leaf</v>
-      </c>
-      <c r="V1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP_twigs</v>
-      </c>
-      <c r="W1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP_flower</v>
-      </c>
-      <c r="X1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP_fruit</v>
-      </c>
-      <c r="Y1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP_unidentified</v>
-      </c>
-      <c r="Z1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP_seed</v>
-      </c>
-      <c r="AA1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP_herbivory</v>
-      </c>
-      <c r="AB1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP_branch_turnover</v>
-      </c>
-      <c r="AC1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPPacw_10cm_big_stem</v>
-      </c>
-      <c r="AD1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPPacw_small_stem</v>
-      </c>
-      <c r="AE1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP_all_stem</v>
-      </c>
-      <c r="AF1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP_coarseroot</v>
-      </c>
-      <c r="AG1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP_fineroot</v>
-      </c>
-      <c r="AH1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP_herbs</v>
-      </c>
-      <c r="AI1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP_AG</v>
-      </c>
-      <c r="AJ1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP_BG</v>
-      </c>
-      <c r="AK1" t="str">
-        <f t="shared" si="0"/>
-        <v>dNPP</v>
+      <c r="T1" t="s">
+        <v>99</v>
+      </c>
+      <c r="U1" t="s">
+        <v>100</v>
+      </c>
+      <c r="V1" t="s">
+        <v>101</v>
+      </c>
+      <c r="W1" t="s">
+        <v>102</v>
+      </c>
+      <c r="X1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>